<commit_message>
EPBDS-13292 Tests with hierarchy of Error datatype
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/junit/EPBDS-12729_error_code_message.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/junit/EPBDS-12729_error_code_message.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="79">
   <si>
     <t xml:space="preserve">Spreadsheet SpreadsheetResult error1()</t>
   </si>
@@ -158,6 +158,105 @@
   </si>
   <si>
     <t xml:space="preserve">Test error4 error4_test5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet SpreadsheetResult error5()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test error5 error5_test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_res_.$Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_error_.msg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_error_.base.code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_error_.base.msg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_error_.nested[0].code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_error_.nested[0].msg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_error_.nested[1].code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_error_.nested[1].msg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=Error(msg="base", code = 17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_res_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=Error(msg="x1", code = 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=Error(msg="x2", code = 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not achieved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=add($x1, $x2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=new Error("total", 42, $nested, $base)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">= error($error)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datatype Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error[]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error</t>
   </si>
 </sst>
 </file>
@@ -268,26 +367,26 @@
   </sheetPr>
   <dimension ref="C4:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F82" activeCellId="0" sqref="F82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="8.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="8.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="8.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.16"/>
@@ -1163,11 +1262,477 @@
       <c r="W62" s="3"/>
       <c r="X62" s="3"/>
     </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="F64" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C65" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L65" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="M65" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N65" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O65" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L66" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="M66" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N66" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O66" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J69" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K69" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="L69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M69" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="N69" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O69" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K70" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M70" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="N70" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O70" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="J71" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K71" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="L71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M71" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="N71" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O71" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H72" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="K72" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="L72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M72" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="N72" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O72" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F73" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J73" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="L73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M73" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="N73" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O73" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F74" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J74" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K74" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="M74" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="N74" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O74" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F75" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J75" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K75" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="L75" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N75" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O75" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C76" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H76" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I76" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J76" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K76" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="L76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M76" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="O76" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H77" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I77" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J77" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K77" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="L77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M77" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="N77" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H78" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I78" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J78" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K78" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="L78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M78" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C79" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H79" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I79" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J79" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K79" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C80" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H80" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I80" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F81" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F82" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I82" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="J4:K4"/>
@@ -1186,6 +1751,8 @@
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="P52:S52"/>
     <mergeCell ref="U62:X62"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="F64:G64"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>